<commit_message>
fixees t o pca plot
</commit_message>
<xml_diff>
--- a/res_table.xlsx
+++ b/res_table.xlsx
@@ -488,16 +488,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>2.875295965000987</v>
+        <v>2.471608527004719</v>
       </c>
       <c r="E2" t="n">
-        <v>3.538097381591797</v>
+        <v>3.410691294819117</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4376479825004935</v>
+        <v>0.2358042635023594</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7690486907958984</v>
+        <v>0.7053456474095583</v>
       </c>
       <c r="H2" t="n">
         <v>0.1637372076511383</v>
@@ -519,16 +519,16 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>3.064127828925848</v>
+        <v>2.338538888841867</v>
       </c>
       <c r="E3" t="n">
-        <v>2.913406528532505</v>
+        <v>2.43381213163957</v>
       </c>
       <c r="F3" t="n">
-        <v>0.532063914462924</v>
+        <v>0.1692694444209337</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4567032642662525</v>
+        <v>0.216906065819785</v>
       </c>
       <c r="H3" t="n">
         <v>0.3606675863265991</v>
@@ -550,16 +550,16 @@
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>4.554968928918242</v>
+        <v>4.675471302121878</v>
       </c>
       <c r="E4" t="n">
-        <v>5.002135161310434</v>
+        <v>4.276767794974148</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1387422322295606</v>
+        <v>0.1688678255304694</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2505337903276086</v>
+        <v>0.06919194874353707</v>
       </c>
       <c r="H4" t="n">
         <v>0.006818106397986412</v>
@@ -581,16 +581,16 @@
         <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>5.814834922552109</v>
+        <v>5.168602275429294</v>
       </c>
       <c r="E5" t="n">
-        <v>5.531789172440767</v>
+        <v>5.393329305574298</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1629669845104217</v>
+        <v>0.03372045508585871</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1063578344881535</v>
+        <v>0.07866586111485958</v>
       </c>
       <c r="H5" t="n">
         <v>0.006897940766066313</v>
@@ -612,16 +612,16 @@
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>3.440532090142369</v>
+        <v>3.855129688978195</v>
       </c>
       <c r="E6" t="n">
-        <v>3.539059318602085</v>
+        <v>3.243498809635639</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1468440300474564</v>
+        <v>0.2850432296593984</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1796864395340284</v>
+        <v>0.0811662698785464</v>
       </c>
       <c r="H6" t="n">
         <v>0.008187552914023399</v>
@@ -643,16 +643,16 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>2.667594781145453</v>
+        <v>2.411616187542677</v>
       </c>
       <c r="E7" t="n">
-        <v>2.227042407728732</v>
+        <v>2.285308588296175</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3337973905727267</v>
+        <v>0.2058080937713385</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1135212038643658</v>
+        <v>0.1426542941480875</v>
       </c>
       <c r="H7" t="n">
         <v>0.008930059149861336</v>
@@ -674,16 +674,16 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>4.500956184230745</v>
+        <v>4.397048187442124</v>
       </c>
       <c r="E8" t="n">
-        <v>4.364407908171415</v>
+        <v>4.716597873717546</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1252390460576862</v>
+        <v>0.09926204686053097</v>
       </c>
       <c r="G8" t="n">
-        <v>0.09110197704285383</v>
+        <v>0.1791494684293866</v>
       </c>
       <c r="H8" t="n">
         <v>0.006495729554444551</v>
@@ -705,16 +705,16 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2.511299774050713</v>
+        <v>2.329123958013952</v>
       </c>
       <c r="E9" t="n">
-        <v>2.883997913450003</v>
+        <v>2.737986572086811</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2556498870253563</v>
+        <v>0.1645619790069759</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4419989567250013</v>
+        <v>0.3689932860434055</v>
       </c>
       <c r="H9" t="n">
         <v>0.006429604254662991</v>
@@ -736,16 +736,16 @@
         <v>3</v>
       </c>
       <c r="D10" t="n">
-        <v>3.413410508073866</v>
+        <v>4.394832290709019</v>
       </c>
       <c r="E10" t="n">
-        <v>3.997776806354523</v>
+        <v>3.822696465998888</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1378035026912888</v>
+        <v>0.4649440969030063</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3325922687848409</v>
+        <v>0.2742321553329627</v>
       </c>
       <c r="H10" t="n">
         <v>0.009470631368458271</v>
@@ -767,16 +767,16 @@
         <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>3.71144193969667</v>
+        <v>3.868999440222979</v>
       </c>
       <c r="E11" t="n">
-        <v>3.499153878539801</v>
+        <v>3.620934154838324</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2371473132322232</v>
+        <v>0.2896664800743262</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1663846261799335</v>
+        <v>0.2069780516127745</v>
       </c>
       <c r="H11" t="n">
         <v>0.01107843872159719</v>
@@ -798,16 +798,16 @@
         <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>3.724961582571268</v>
+        <v>3.50879477057606</v>
       </c>
       <c r="E12" t="n">
-        <v>3.195607740432024</v>
+        <v>3.620779767632484</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2416538608570894</v>
+        <v>0.1695982568586866</v>
       </c>
       <c r="G12" t="n">
-        <v>0.065202580144008</v>
+        <v>0.2069265892108282</v>
       </c>
       <c r="H12" t="n">
         <v>0.04844946414232254</v>
@@ -829,16 +829,16 @@
         <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>4.476688546128571</v>
+        <v>4.320871399249882</v>
       </c>
       <c r="E13" t="n">
-        <v>4.632588542997837</v>
+        <v>4.570783686824143</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1191721365321428</v>
+        <v>0.08021784981247038</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1581471357494593</v>
+        <v>0.1426959217060357</v>
       </c>
       <c r="H13" t="n">
         <v>0.008696182630956173</v>
@@ -860,16 +860,16 @@
         <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>3.621022529900074</v>
+        <v>3.01353463344276</v>
       </c>
       <c r="E14" t="n">
-        <v>2.789534740149975</v>
+        <v>2.814172249287367</v>
       </c>
       <c r="F14" t="n">
-        <v>0.810511264950037</v>
+        <v>0.5067673167213798</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3947673700749874</v>
+        <v>0.4070861246436834</v>
       </c>
       <c r="H14" t="n">
         <v>0.2578360438346863</v>
@@ -891,16 +891,16 @@
         <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>3.389196217060089</v>
+        <v>3.618761103600264</v>
       </c>
       <c r="E15" t="n">
-        <v>3.538676145486534</v>
+        <v>3.926798224449158</v>
       </c>
       <c r="F15" t="n">
-        <v>0.129732072353363</v>
+        <v>0.2062537012000879</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1795587151621779</v>
+        <v>0.3089327414830526</v>
       </c>
       <c r="H15" t="n">
         <v>0.09630544483661652</v>

</xml_diff>